<commit_message>
[Snehil] Add : Retreive data from flipkart using work queue
</commit_message>
<xml_diff>
--- a/flipkart product details.xlsx
+++ b/flipkart product details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snehil\Desktop\FlipkartAutomation-BluePrism\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51F4A6E-70DE-4FF6-AD58-AE2F96097D5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAEED58-C2B9-4ACE-9B90-8605DD18C3EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3130" yWindow="1630" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
@@ -70,6 +70,27 @@
   </si>
   <si>
     <t>Apple iPhone 11 (Green, 128 GB) (Includes EarPods, Power Adapter)</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Purple</t>
   </si>
 </sst>
 </file>
@@ -387,13 +408,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,8 +426,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -414,8 +440,11 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -425,8 +454,11 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -436,8 +468,11 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -447,8 +482,11 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -458,8 +496,11 @@
       <c r="C6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -469,8 +510,11 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -480,8 +524,11 @@
       <c r="C8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -491,8 +538,11 @@
       <c r="C9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -502,8 +552,11 @@
       <c r="C10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -512,6 +565,9 @@
       </c>
       <c r="C11" t="s">
         <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>